<commit_message>
Read data from Excel. Part 3 (EPPlus realization improved)
</commit_message>
<xml_diff>
--- a/FitMeApp/wwwroot/ExcelFiles/Import/BigRock/VisitorsChart.xlsx
+++ b/FitMeApp/wwwroot/ExcelFiles/Import/BigRock/VisitorsChart.xlsx
@@ -25,7 +25,7 @@
     <t>Wednesday</t>
   </si>
   <si>
-    <t>Thurthday</t>
+    <t>Thursday</t>
   </si>
   <si>
     <t>Friday</t>
@@ -1729,6 +1729,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:N1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
@@ -1736,7 +1737,6 @@
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>